<commit_message>
Update README.md, gitignore, tekken_scrap.py, Add Yoshimitsu data
</commit_message>
<xml_diff>
--- a/data/asuka-kazama-tekken-8-frame-data.xlsx
+++ b/data/asuka-kazama-tekken-8-frame-data.xlsx
@@ -492,15 +492,11 @@
       <c r="D2" t="n">
         <v>10</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>+9</t>
-        </is>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>9</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -526,15 +522,11 @@
       <c r="D3" t="n">
         <v>10</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>-7</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>+4</t>
-        </is>
+      <c r="E3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -560,15 +552,11 @@
       <c r="D4" t="n">
         <v>10</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>-8</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>+3</t>
-        </is>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -594,15 +582,11 @@
       <c r="D5" t="n">
         <v>10</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Knockdown</t>
-        </is>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>70</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -628,15 +612,11 @@
       <c r="D6" t="n">
         <v>10</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-18</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>-7</t>
-        </is>
+      <c r="E6" t="n">
+        <v>18</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-7</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -662,15 +642,11 @@
       <c r="D7" t="n">
         <v>10</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>-12</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Knockdown</t>
-        </is>
+      <c r="E7" t="n">
+        <v>12</v>
+      </c>
+      <c r="F7" t="n">
+        <v>70</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -696,15 +672,11 @@
       <c r="D8" t="n">
         <v>10</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E8" t="n">
+        <v>11</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -730,15 +702,11 @@
       <c r="D9" t="n">
         <v>10</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E9" t="n">
+        <v>11</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -764,15 +732,11 @@
       <c r="D10" t="n">
         <v>10</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E10" t="n">
+        <v>11</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -798,15 +762,11 @@
       <c r="D11" t="n">
         <v>12</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E11" t="n">
+        <v>11</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -832,15 +792,11 @@
       <c r="D12" t="n">
         <v>12</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>-3</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>+8</t>
-        </is>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -867,10 +823,8 @@
         <v>12</v>
       </c>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Knockdown</t>
-        </is>
+      <c r="F13" t="n">
+        <v>70</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
@@ -896,15 +850,11 @@
       <c r="D14" t="n">
         <v>12</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>-10</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>+3</t>
-        </is>
+      <c r="E14" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" t="n">
+        <v>3</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -982,15 +932,11 @@
       <c r="D17" t="n">
         <v>12</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>-19</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Knockdown</t>
-        </is>
+      <c r="E17" t="n">
+        <v>19</v>
+      </c>
+      <c r="F17" t="n">
+        <v>70</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1016,15 +962,11 @@
       <c r="D18" t="n">
         <v>14</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>-7</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>+9</t>
-        </is>
+      <c r="E18" t="n">
+        <v>7</v>
+      </c>
+      <c r="F18" t="n">
+        <v>9</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1050,15 +992,11 @@
       <c r="D19" t="n">
         <v>14</v>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>+8</t>
-        </is>
+      <c r="E19" t="n">
+        <v>11</v>
+      </c>
+      <c r="F19" t="n">
+        <v>8</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,15 +1022,11 @@
       <c r="D20" t="n">
         <v>11</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>-7</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>+7</t>
-        </is>
+      <c r="E20" t="n">
+        <v>7</v>
+      </c>
+      <c r="F20" t="n">
+        <v>7</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1118,15 +1052,11 @@
       <c r="D21" t="n">
         <v>16</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Knockdown</t>
-        </is>
+      <c r="E21" t="n">
+        <v>9</v>
+      </c>
+      <c r="F21" t="n">
+        <v>70</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1152,15 +1082,11 @@
       <c r="D22" t="n">
         <v>23</v>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>-6</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E22" t="n">
+        <v>6</v>
+      </c>
+      <c r="F22" t="n">
+        <v>70</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1186,15 +1112,11 @@
       <c r="D23" t="n">
         <v>23</v>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>-6</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E23" t="n">
+        <v>6</v>
+      </c>
+      <c r="F23" t="n">
+        <v>70</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1220,15 +1142,11 @@
       <c r="D24" t="n">
         <v>14</v>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>-19</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>-8</t>
-        </is>
+      <c r="E24" t="n">
+        <v>19</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-8</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1254,15 +1172,11 @@
       <c r="D25" t="n">
         <v>14</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>+9</t>
-        </is>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="n">
+        <v>9</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1288,15 +1202,11 @@
       <c r="D26" t="n">
         <v>14</v>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>+4</t>
-        </is>
+      <c r="E26" t="n">
+        <v>9</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1322,16 +1232,10 @@
       <c r="D27" t="n">
         <v>14</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">-23	</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">KDN	</t>
-        </is>
-      </c>
+      <c r="E27" t="n">
+        <v>23</v>
+      </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
           <t xml:space="preserve">KDN	</t>
@@ -1356,16 +1260,10 @@
       <c r="D28" t="n">
         <v>14</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">-2	</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">KDN	</t>
-        </is>
-      </c>
+      <c r="E28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
           <t xml:space="preserve">KDN	</t>
@@ -1390,15 +1288,11 @@
       <c r="D29" t="n">
         <v>14</v>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">-37	</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">-26	</t>
-        </is>
+      <c r="E29" t="n">
+        <v>37</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-26</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1424,15 +1318,11 @@
       <c r="D30" t="n">
         <v>17</v>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>-18</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E30" t="n">
+        <v>18</v>
+      </c>
+      <c r="F30" t="n">
+        <v>70</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1508,15 +1398,11 @@
       <c r="D33" t="n">
         <v>31</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E33" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" t="n">
+        <v>70</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1566,15 +1452,11 @@
       <c r="D35" t="n">
         <v>52</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>+6</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E35" t="n">
+        <v>-6</v>
+      </c>
+      <c r="F35" t="n">
+        <v>70</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1604,15 +1486,9 @@
       <c r="D36" t="n">
         <v>70</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="n">
+        <v>70</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -1638,15 +1514,11 @@
       <c r="D37" t="n">
         <v>19</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>+3</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E37" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F37" t="n">
+        <v>70</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1676,15 +1548,11 @@
       <c r="D38" t="n">
         <v>15</v>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E38" t="n">
+        <v>9</v>
+      </c>
+      <c r="F38" t="n">
+        <v>70</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1715,10 +1583,8 @@
         <v>29</v>
       </c>
       <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="F39" t="n">
+        <v>70</v>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
@@ -1740,15 +1606,11 @@
       <c r="D40" t="n">
         <v>23</v>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>70</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1774,15 +1636,11 @@
       <c r="D41" t="n">
         <v>13</v>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>-3</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>+8</t>
-        </is>
+      <c r="E41" t="n">
+        <v>3</v>
+      </c>
+      <c r="F41" t="n">
+        <v>8</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -1808,15 +1666,11 @@
       <c r="D42" t="n">
         <v>13</v>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>TH</t>
-        </is>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" t="n">
+        <v>70</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1842,15 +1696,11 @@
       <c r="D43" t="n">
         <v>13</v>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>-12</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E43" t="n">
+        <v>12</v>
+      </c>
+      <c r="F43" t="n">
+        <v>70</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1876,15 +1726,11 @@
       <c r="D44" t="n">
         <v>15</v>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>-6</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E44" t="n">
+        <v>6</v>
+      </c>
+      <c r="F44" t="n">
+        <v>70</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1910,15 +1756,11 @@
       <c r="D45" t="n">
         <v>20</v>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>-8</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E45" t="n">
+        <v>8</v>
+      </c>
+      <c r="F45" t="n">
+        <v>70</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1944,15 +1786,11 @@
       <c r="D46" t="n">
         <v>12</v>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
+      <c r="E46" t="n">
+        <v>9</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1978,15 +1816,11 @@
       <c r="D47" t="n">
         <v>28</v>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>-26</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E47" t="n">
+        <v>26</v>
+      </c>
+      <c r="F47" t="n">
+        <v>70</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2032,15 +1866,11 @@
       <c r="D49" t="n">
         <v>10</v>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>-5</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>+6</t>
-        </is>
+      <c r="E49" t="n">
+        <v>5</v>
+      </c>
+      <c r="F49" t="n">
+        <v>6</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2092,15 +1922,11 @@
       <c r="D51" t="n">
         <v>18</v>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>-4</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>+9</t>
-        </is>
+      <c r="E51" t="n">
+        <v>4</v>
+      </c>
+      <c r="F51" t="n">
+        <v>9</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2126,15 +1952,11 @@
       <c r="D52" t="n">
         <v>16</v>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>-17</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>-3</t>
-        </is>
+      <c r="E52" t="n">
+        <v>17</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-3</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2160,15 +1982,11 @@
       <c r="D53" t="n">
         <v>12</v>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>-13</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
+      <c r="E53" t="n">
+        <v>13</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-2</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2194,15 +2012,11 @@
       <c r="D54" t="n">
         <v>20</v>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>-18</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E54" t="n">
+        <v>18</v>
+      </c>
+      <c r="F54" t="n">
+        <v>70</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2228,15 +2042,11 @@
       <c r="D55" t="n">
         <v>14</v>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>-25</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E55" t="n">
+        <v>25</v>
+      </c>
+      <c r="F55" t="n">
+        <v>70</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2262,15 +2072,11 @@
       <c r="D56" t="n">
         <v>14</v>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>+7</t>
-        </is>
+      <c r="E56" t="n">
+        <v>9</v>
+      </c>
+      <c r="F56" t="n">
+        <v>7</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -2322,15 +2128,11 @@
       <c r="D58" t="n">
         <v>14</v>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E58" t="n">
+        <v>9</v>
+      </c>
+      <c r="F58" t="n">
+        <v>70</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2357,10 +2159,8 @@
         <v>14</v>
       </c>
       <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="F59" t="n">
+        <v>70</v>
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
@@ -2382,15 +2182,11 @@
       <c r="D60" t="n">
         <v>20</v>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E60" t="n">
+        <v>11</v>
+      </c>
+      <c r="F60" t="n">
+        <v>70</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2416,15 +2212,11 @@
       <c r="D61" t="n">
         <v>20</v>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>-12</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>+4</t>
-        </is>
+      <c r="E61" t="n">
+        <v>12</v>
+      </c>
+      <c r="F61" t="n">
+        <v>4</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2451,10 +2243,8 @@
         <v>42</v>
       </c>
       <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="F62" t="n">
+        <v>70</v>
       </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
@@ -2480,15 +2270,11 @@
       <c r="D63" t="n">
         <v>29</v>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>-10</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>+6</t>
-        </is>
+      <c r="E63" t="n">
+        <v>10</v>
+      </c>
+      <c r="F63" t="n">
+        <v>6</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2538,15 +2324,11 @@
       <c r="D65" t="n">
         <v>15</v>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>-4</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>+1</t>
-        </is>
+      <c r="E65" t="n">
+        <v>4</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2572,15 +2354,11 @@
       <c r="D66" t="n">
         <v>15</v>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>-7</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>+4</t>
-        </is>
+      <c r="E66" t="n">
+        <v>7</v>
+      </c>
+      <c r="F66" t="n">
+        <v>4</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2606,15 +2384,11 @@
       <c r="D67" t="n">
         <v>15</v>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E67" t="n">
+        <v>11</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -2640,15 +2414,11 @@
       <c r="D68" t="n">
         <v>15</v>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E68" t="n">
+        <v>11</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2678,15 +2448,11 @@
       <c r="D69" t="n">
         <v>36</v>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
+      <c r="E69" t="n">
+        <v>9</v>
+      </c>
+      <c r="F69" t="n">
+        <v>2</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2712,15 +2478,11 @@
       <c r="D70" t="n">
         <v>46</v>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>-6</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
+      <c r="E70" t="n">
+        <v>6</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-1</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2746,15 +2508,11 @@
       <c r="D71" t="n">
         <v>46</v>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>-13</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E71" t="n">
+        <v>13</v>
+      </c>
+      <c r="F71" t="n">
+        <v>70</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2780,15 +2538,11 @@
       <c r="D72" t="n">
         <v>16</v>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>-19</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E72" t="n">
+        <v>19</v>
+      </c>
+      <c r="F72" t="n">
+        <v>70</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2814,15 +2568,11 @@
       <c r="D73" t="n">
         <v>16</v>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>-20</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E73" t="n">
+        <v>20</v>
+      </c>
+      <c r="F73" t="n">
+        <v>70</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2848,15 +2598,11 @@
       <c r="D74" t="n">
         <v>16</v>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>-33</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E74" t="n">
+        <v>33</v>
+      </c>
+      <c r="F74" t="n">
+        <v>70</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2883,10 +2629,8 @@
         <v>16</v>
       </c>
       <c r="E75" t="inlineStr"/>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="F75" t="n">
+        <v>70</v>
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
@@ -2908,15 +2652,11 @@
       <c r="D76" t="n">
         <v>16</v>
       </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E76" t="n">
+        <v>11</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2942,15 +2682,11 @@
       <c r="D77" t="n">
         <v>16</v>
       </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E77" t="n">
+        <v>11</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2976,15 +2712,11 @@
       <c r="D78" t="n">
         <v>15</v>
       </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>-7</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>+8</t>
-        </is>
+      <c r="E78" t="n">
+        <v>7</v>
+      </c>
+      <c r="F78" t="n">
+        <v>8</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3010,15 +2742,11 @@
       <c r="D79" t="n">
         <v>15</v>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>-12</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>+4</t>
-        </is>
+      <c r="E79" t="n">
+        <v>12</v>
+      </c>
+      <c r="F79" t="n">
+        <v>4</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3044,15 +2772,11 @@
       <c r="D80" t="n">
         <v>15</v>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>-16</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E80" t="n">
+        <v>16</v>
+      </c>
+      <c r="F80" t="n">
+        <v>70</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3079,10 +2803,8 @@
         <v>15</v>
       </c>
       <c r="E81" t="inlineStr"/>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="F81" t="n">
+        <v>70</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3108,15 +2830,11 @@
       <c r="D82" t="n">
         <v>12</v>
       </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>-8</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>+5</t>
-        </is>
+      <c r="E82" t="n">
+        <v>8</v>
+      </c>
+      <c r="F82" t="n">
+        <v>5</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -3142,15 +2860,11 @@
       <c r="D83" t="n">
         <v>12</v>
       </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>-13</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
+      <c r="E83" t="n">
+        <v>13</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-2</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -3176,15 +2890,11 @@
       <c r="D84" t="n">
         <v>12</v>
       </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>-14</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>+5</t>
-        </is>
+      <c r="E84" t="n">
+        <v>14</v>
+      </c>
+      <c r="F84" t="n">
+        <v>5</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3210,15 +2920,11 @@
       <c r="D85" t="n">
         <v>24</v>
       </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>+6</t>
-        </is>
+      <c r="E85" t="n">
+        <v>9</v>
+      </c>
+      <c r="F85" t="n">
+        <v>6</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -3244,15 +2950,11 @@
       <c r="D86" t="n">
         <v>18</v>
       </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>-12</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
+      <c r="E86" t="n">
+        <v>12</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-1</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3278,15 +2980,11 @@
       <c r="D87" t="n">
         <v>15</v>
       </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>-12</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>+9</t>
-        </is>
+      <c r="E87" t="n">
+        <v>12</v>
+      </c>
+      <c r="F87" t="n">
+        <v>9</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3312,15 +3010,11 @@
       <c r="D88" t="n">
         <v>14</v>
       </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>-17</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>TH</t>
-        </is>
+      <c r="E88" t="n">
+        <v>17</v>
+      </c>
+      <c r="F88" t="n">
+        <v>70</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -3346,15 +3040,11 @@
       <c r="D89" t="n">
         <v>20</v>
       </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>-3</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>+8</t>
-        </is>
+      <c r="E89" t="n">
+        <v>3</v>
+      </c>
+      <c r="F89" t="n">
+        <v>8</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -3380,15 +3070,11 @@
       <c r="D90" t="n">
         <v>20</v>
       </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>-15</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E90" t="n">
+        <v>15</v>
+      </c>
+      <c r="F90" t="n">
+        <v>70</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -3414,15 +3100,11 @@
       <c r="D91" t="n">
         <v>20</v>
       </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>-13</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E91" t="n">
+        <v>13</v>
+      </c>
+      <c r="F91" t="n">
+        <v>70</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3449,10 +3131,8 @@
         <v>31</v>
       </c>
       <c r="E92" t="inlineStr"/>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="F92" t="n">
+        <v>70</v>
       </c>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="inlineStr">
@@ -3479,10 +3159,8 @@
         <v>31</v>
       </c>
       <c r="E93" t="inlineStr"/>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="F93" t="n">
+        <v>70</v>
       </c>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="inlineStr"/>
@@ -3504,15 +3182,11 @@
       <c r="D94" t="n">
         <v>25</v>
       </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E94" t="n">
+        <v>9</v>
+      </c>
+      <c r="F94" t="n">
+        <v>70</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -3538,15 +3212,11 @@
       <c r="D95" t="n">
         <v>68</v>
       </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>70</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3572,10 +3242,8 @@
       <c r="D96" t="n">
         <v>23</v>
       </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>+4</t>
-        </is>
+      <c r="E96" t="n">
+        <v>-4</v>
       </c>
       <c r="F96" t="inlineStr"/>
       <c r="G96" t="inlineStr">
@@ -3602,15 +3270,11 @@
       <c r="D97" t="n">
         <v>15</v>
       </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>-13</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>-3</t>
-        </is>
+      <c r="E97" t="n">
+        <v>13</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-3</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3636,15 +3300,11 @@
       <c r="D98" t="n">
         <v>15</v>
       </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>-5</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E98" t="n">
+        <v>5</v>
+      </c>
+      <c r="F98" t="n">
+        <v>70</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3670,15 +3330,11 @@
       <c r="D99" t="n">
         <v>15</v>
       </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>-8</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E99" t="n">
+        <v>8</v>
+      </c>
+      <c r="F99" t="n">
+        <v>70</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -3705,10 +3361,8 @@
         <v>15</v>
       </c>
       <c r="E100" t="inlineStr"/>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="F100" t="n">
+        <v>70</v>
       </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="inlineStr"/>
@@ -3730,15 +3384,11 @@
       <c r="D101" t="n">
         <v>20</v>
       </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>+11</t>
-        </is>
+      <c r="E101" t="n">
+        <v>9</v>
+      </c>
+      <c r="F101" t="n">
+        <v>11</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -3764,15 +3414,11 @@
       <c r="D102" t="n">
         <v>20</v>
       </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>+11</t>
-        </is>
+      <c r="E102" t="n">
+        <v>9</v>
+      </c>
+      <c r="F102" t="n">
+        <v>11</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -3798,15 +3444,11 @@
       <c r="D103" t="n">
         <v>20</v>
       </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>-3</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E103" t="n">
+        <v>3</v>
+      </c>
+      <c r="F103" t="n">
+        <v>70</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -3833,10 +3475,8 @@
         <v>19</v>
       </c>
       <c r="E104" t="inlineStr"/>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="F104" t="n">
+        <v>70</v>
       </c>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="inlineStr"/>
@@ -3858,15 +3498,11 @@
       <c r="D105" t="n">
         <v>24</v>
       </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
+      <c r="F105" t="n">
+        <v>70</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -3893,10 +3529,8 @@
         <v>17</v>
       </c>
       <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="F106" t="n">
+        <v>70</v>
       </c>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="inlineStr"/>
@@ -3918,15 +3552,11 @@
       <c r="D107" t="n">
         <v>10</v>
       </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>-5</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>+6</t>
-        </is>
+      <c r="E107" t="n">
+        <v>5</v>
+      </c>
+      <c r="F107" t="n">
+        <v>6</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
@@ -3952,15 +3582,11 @@
       <c r="D108" t="n">
         <v>11</v>
       </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>-4</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>+7</t>
-        </is>
+      <c r="E108" t="n">
+        <v>4</v>
+      </c>
+      <c r="F108" t="n">
+        <v>7</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
@@ -3986,15 +3612,11 @@
       <c r="D109" t="n">
         <v>16</v>
       </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>-17</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>-3</t>
-        </is>
+      <c r="E109" t="n">
+        <v>17</v>
+      </c>
+      <c r="F109" t="n">
+        <v>-3</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -4020,15 +3642,11 @@
       <c r="D110" t="n">
         <v>12</v>
       </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>-15</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>-4</t>
-        </is>
+      <c r="E110" t="n">
+        <v>15</v>
+      </c>
+      <c r="F110" t="n">
+        <v>-4</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -4054,15 +3672,11 @@
       <c r="D111" t="n">
         <v>21</v>
       </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>-6</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>+5</t>
-        </is>
+      <c r="E111" t="n">
+        <v>6</v>
+      </c>
+      <c r="F111" t="n">
+        <v>5</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -4088,15 +3702,11 @@
       <c r="D112" t="n">
         <v>21</v>
       </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>70</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
@@ -4122,15 +3732,11 @@
       <c r="D113" t="n">
         <v>21</v>
       </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E113" t="n">
+        <v>0</v>
+      </c>
+      <c r="F113" t="n">
+        <v>70</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -4156,15 +3762,11 @@
       <c r="D114" t="n">
         <v>14</v>
       </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>-7</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>+4</t>
-        </is>
+      <c r="E114" t="n">
+        <v>7</v>
+      </c>
+      <c r="F114" t="n">
+        <v>4</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
@@ -4190,15 +3792,11 @@
       <c r="D115" t="n">
         <v>14</v>
       </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>-8</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E115" t="n">
+        <v>8</v>
+      </c>
+      <c r="F115" t="n">
+        <v>70</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -4224,15 +3822,11 @@
       <c r="D116" t="n">
         <v>13</v>
       </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>-8</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>+8</t>
-        </is>
+      <c r="E116" t="n">
+        <v>8</v>
+      </c>
+      <c r="F116" t="n">
+        <v>8</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -4258,15 +3852,11 @@
       <c r="D117" t="n">
         <v>13</v>
       </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>+9</t>
-        </is>
+      <c r="E117" t="n">
+        <v>2</v>
+      </c>
+      <c r="F117" t="n">
+        <v>9</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -4293,10 +3883,8 @@
         <v>13</v>
       </c>
       <c r="E118" t="inlineStr"/>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>Th</t>
-        </is>
+      <c r="F118" t="n">
+        <v>70</v>
       </c>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
@@ -4318,15 +3906,11 @@
       <c r="D119" t="n">
         <v>18</v>
       </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>-16</t>
-        </is>
-      </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E119" t="n">
+        <v>16</v>
+      </c>
+      <c r="F119" t="n">
+        <v>70</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -4352,15 +3936,11 @@
       <c r="D120" t="n">
         <v>11</v>
       </c>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>-3</t>
-        </is>
-      </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>+8</t>
-        </is>
+      <c r="E120" t="n">
+        <v>3</v>
+      </c>
+      <c r="F120" t="n">
+        <v>8</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -4386,15 +3966,11 @@
       <c r="D121" t="n">
         <v>21</v>
       </c>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
-      </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>+13</t>
-        </is>
+      <c r="E121" t="n">
+        <v>2</v>
+      </c>
+      <c r="F121" t="n">
+        <v>13</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -4420,15 +3996,11 @@
       <c r="D122" t="n">
         <v>16</v>
       </c>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E122" t="n">
+        <v>11</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
@@ -4454,15 +4026,11 @@
       <c r="D123" t="n">
         <v>17</v>
       </c>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>-9</t>
-        </is>
-      </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E123" t="n">
+        <v>9</v>
+      </c>
+      <c r="F123" t="n">
+        <v>70</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
@@ -4510,15 +4078,11 @@
       <c r="D125" t="n">
         <v>17</v>
       </c>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>-6</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>+7</t>
-        </is>
+      <c r="E125" t="n">
+        <v>6</v>
+      </c>
+      <c r="F125" t="n">
+        <v>7</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -4544,15 +4108,11 @@
       <c r="D126" t="n">
         <v>20</v>
       </c>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>-7</t>
-        </is>
-      </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>+4</t>
-        </is>
+      <c r="E126" t="n">
+        <v>7</v>
+      </c>
+      <c r="F126" t="n">
+        <v>4</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
@@ -4578,15 +4138,11 @@
       <c r="D127" t="n">
         <v>20</v>
       </c>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>-25</t>
-        </is>
-      </c>
-      <c r="F127" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E127" t="n">
+        <v>25</v>
+      </c>
+      <c r="F127" t="n">
+        <v>70</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -4612,15 +4168,11 @@
       <c r="D128" t="n">
         <v>20</v>
       </c>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t>-26</t>
-        </is>
-      </c>
-      <c r="F128" t="inlineStr">
-        <is>
-          <t>KDN</t>
-        </is>
+      <c r="E128" t="n">
+        <v>26</v>
+      </c>
+      <c r="F128" t="n">
+        <v>70</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -4646,15 +4198,11 @@
       <c r="D129" t="n">
         <v>20</v>
       </c>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>-26</t>
-        </is>
-      </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>-15</t>
-        </is>
+      <c r="E129" t="n">
+        <v>26</v>
+      </c>
+      <c r="F129" t="n">
+        <v>-15</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
@@ -4680,15 +4228,11 @@
       <c r="D130" t="n">
         <v>22</v>
       </c>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F130" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E130" t="n">
+        <v>11</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
@@ -4714,15 +4258,11 @@
       <c r="D131" t="n">
         <v>22</v>
       </c>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F131" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E131" t="n">
+        <v>11</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
@@ -4748,15 +4288,11 @@
       <c r="D132" t="n">
         <v>22</v>
       </c>
-      <c r="E132" t="inlineStr">
-        <is>
-          <t>-7</t>
-        </is>
-      </c>
-      <c r="F132" t="inlineStr">
-        <is>
-          <t>+4</t>
-        </is>
+      <c r="E132" t="n">
+        <v>7</v>
+      </c>
+      <c r="F132" t="n">
+        <v>4</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
@@ -4782,15 +4318,11 @@
       <c r="D133" t="n">
         <v>22</v>
       </c>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E133" t="n">
+        <v>11</v>
+      </c>
+      <c r="F133" t="n">
+        <v>0</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
@@ -4816,15 +4348,11 @@
       <c r="D134" t="n">
         <v>22</v>
       </c>
-      <c r="E134" t="inlineStr">
-        <is>
-          <t>-11</t>
-        </is>
-      </c>
-      <c r="F134" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E134" t="n">
+        <v>11</v>
+      </c>
+      <c r="F134" t="n">
+        <v>0</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
@@ -4850,15 +4378,11 @@
       <c r="D135" t="n">
         <v>22</v>
       </c>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>-3</t>
-        </is>
-      </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>Launch</t>
-        </is>
+      <c r="E135" t="n">
+        <v>3</v>
+      </c>
+      <c r="F135" t="n">
+        <v>70</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
@@ -4884,15 +4408,11 @@
       <c r="D136" t="n">
         <v>22</v>
       </c>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>-19</t>
-        </is>
-      </c>
-      <c r="F136" t="inlineStr">
-        <is>
-          <t>+9</t>
-        </is>
+      <c r="E136" t="n">
+        <v>19</v>
+      </c>
+      <c r="F136" t="n">
+        <v>9</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update gitignore, tekken_scrap.py, data
</commit_message>
<xml_diff>
--- a/data/asuka-kazama-tekken-8-frame-data.xlsx
+++ b/data/asuka-kazama-tekken-8-frame-data.xlsx
@@ -493,7 +493,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="F2" t="n">
         <v>9</v>
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="F3" t="n">
         <v>4</v>
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="F4" t="n">
         <v>3</v>
@@ -583,7 +583,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="F5" t="n">
         <v>70</v>
@@ -613,7 +613,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>18</v>
+        <v>-18</v>
       </c>
       <c r="F6" t="n">
         <v>-7</v>
@@ -643,7 +643,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="F7" t="n">
         <v>70</v>
@@ -673,7 +673,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -703,7 +703,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -733,7 +733,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -763,7 +763,7 @@
         <v>12</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -793,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="F12" t="n">
         <v>8</v>
@@ -851,7 +851,7 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="F14" t="n">
         <v>3</v>
@@ -933,7 +933,7 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="F17" t="n">
         <v>70</v>
@@ -963,7 +963,7 @@
         <v>14</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="F18" t="n">
         <v>9</v>
@@ -993,7 +993,7 @@
         <v>14</v>
       </c>
       <c r="E19" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F19" t="n">
         <v>8</v>
@@ -1023,7 +1023,7 @@
         <v>11</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="F20" t="n">
         <v>7</v>
@@ -1053,7 +1053,7 @@
         <v>16</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F21" t="n">
         <v>70</v>
@@ -1083,7 +1083,7 @@
         <v>23</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="F22" t="n">
         <v>70</v>
@@ -1113,7 +1113,7 @@
         <v>23</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="F23" t="n">
         <v>70</v>
@@ -1143,7 +1143,7 @@
         <v>14</v>
       </c>
       <c r="E24" t="n">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="F24" t="n">
         <v>-8</v>
@@ -1173,7 +1173,7 @@
         <v>14</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="F25" t="n">
         <v>9</v>
@@ -1203,7 +1203,7 @@
         <v>14</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F26" t="n">
         <v>4</v>
@@ -1233,7 +1233,7 @@
         <v>14</v>
       </c>
       <c r="E27" t="n">
-        <v>23</v>
+        <v>-23</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
@@ -1261,7 +1261,7 @@
         <v>14</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
@@ -1289,7 +1289,7 @@
         <v>14</v>
       </c>
       <c r="E29" t="n">
-        <v>37</v>
+        <v>-37</v>
       </c>
       <c r="F29" t="n">
         <v>-26</v>
@@ -1319,7 +1319,7 @@
         <v>17</v>
       </c>
       <c r="E30" t="n">
-        <v>18</v>
+        <v>-18</v>
       </c>
       <c r="F30" t="n">
         <v>70</v>
@@ -1399,7 +1399,7 @@
         <v>31</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="F33" t="n">
         <v>70</v>
@@ -1453,7 +1453,7 @@
         <v>52</v>
       </c>
       <c r="E35" t="n">
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>70</v>
@@ -1515,7 +1515,7 @@
         <v>19</v>
       </c>
       <c r="E37" t="n">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>70</v>
@@ -1549,7 +1549,7 @@
         <v>15</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F38" t="n">
         <v>70</v>
@@ -1637,7 +1637,7 @@
         <v>13</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="F41" t="n">
         <v>8</v>
@@ -1667,7 +1667,7 @@
         <v>13</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F42" t="n">
         <v>70</v>
@@ -1697,7 +1697,7 @@
         <v>13</v>
       </c>
       <c r="E43" t="n">
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="F43" t="n">
         <v>70</v>
@@ -1727,7 +1727,7 @@
         <v>15</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="F44" t="n">
         <v>70</v>
@@ -1757,7 +1757,7 @@
         <v>20</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="F45" t="n">
         <v>70</v>
@@ -1787,7 +1787,7 @@
         <v>12</v>
       </c>
       <c r="E46" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F46" t="n">
         <v>2</v>
@@ -1817,7 +1817,7 @@
         <v>28</v>
       </c>
       <c r="E47" t="n">
-        <v>26</v>
+        <v>-26</v>
       </c>
       <c r="F47" t="n">
         <v>70</v>
@@ -1867,7 +1867,7 @@
         <v>10</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="F49" t="n">
         <v>6</v>
@@ -1923,7 +1923,7 @@
         <v>18</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="F51" t="n">
         <v>9</v>
@@ -1953,7 +1953,7 @@
         <v>16</v>
       </c>
       <c r="E52" t="n">
-        <v>17</v>
+        <v>-17</v>
       </c>
       <c r="F52" t="n">
         <v>-3</v>
@@ -1983,7 +1983,7 @@
         <v>12</v>
       </c>
       <c r="E53" t="n">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="F53" t="n">
         <v>-2</v>
@@ -2013,7 +2013,7 @@
         <v>20</v>
       </c>
       <c r="E54" t="n">
-        <v>18</v>
+        <v>-18</v>
       </c>
       <c r="F54" t="n">
         <v>70</v>
@@ -2043,7 +2043,7 @@
         <v>14</v>
       </c>
       <c r="E55" t="n">
-        <v>25</v>
+        <v>-25</v>
       </c>
       <c r="F55" t="n">
         <v>70</v>
@@ -2073,7 +2073,7 @@
         <v>14</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F56" t="n">
         <v>7</v>
@@ -2129,7 +2129,7 @@
         <v>14</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F58" t="n">
         <v>70</v>
@@ -2183,7 +2183,7 @@
         <v>20</v>
       </c>
       <c r="E60" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F60" t="n">
         <v>70</v>
@@ -2213,7 +2213,7 @@
         <v>20</v>
       </c>
       <c r="E61" t="n">
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="F61" t="n">
         <v>4</v>
@@ -2271,7 +2271,7 @@
         <v>29</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="F63" t="n">
         <v>6</v>
@@ -2325,7 +2325,7 @@
         <v>15</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="F65" t="n">
         <v>1</v>
@@ -2355,7 +2355,7 @@
         <v>15</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="F66" t="n">
         <v>4</v>
@@ -2385,7 +2385,7 @@
         <v>15</v>
       </c>
       <c r="E67" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
@@ -2415,7 +2415,7 @@
         <v>15</v>
       </c>
       <c r="E68" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F68" t="n">
         <v>0</v>
@@ -2449,7 +2449,7 @@
         <v>36</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F69" t="n">
         <v>2</v>
@@ -2479,7 +2479,7 @@
         <v>46</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="F70" t="n">
         <v>-1</v>
@@ -2509,7 +2509,7 @@
         <v>46</v>
       </c>
       <c r="E71" t="n">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="F71" t="n">
         <v>70</v>
@@ -2539,7 +2539,7 @@
         <v>16</v>
       </c>
       <c r="E72" t="n">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="F72" t="n">
         <v>70</v>
@@ -2569,7 +2569,7 @@
         <v>16</v>
       </c>
       <c r="E73" t="n">
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="F73" t="n">
         <v>70</v>
@@ -2599,7 +2599,7 @@
         <v>16</v>
       </c>
       <c r="E74" t="n">
-        <v>33</v>
+        <v>-33</v>
       </c>
       <c r="F74" t="n">
         <v>70</v>
@@ -2653,7 +2653,7 @@
         <v>16</v>
       </c>
       <c r="E76" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
@@ -2683,7 +2683,7 @@
         <v>16</v>
       </c>
       <c r="E77" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F77" t="n">
         <v>0</v>
@@ -2713,7 +2713,7 @@
         <v>15</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="F78" t="n">
         <v>8</v>
@@ -2743,7 +2743,7 @@
         <v>15</v>
       </c>
       <c r="E79" t="n">
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="F79" t="n">
         <v>4</v>
@@ -2773,7 +2773,7 @@
         <v>15</v>
       </c>
       <c r="E80" t="n">
-        <v>16</v>
+        <v>-16</v>
       </c>
       <c r="F80" t="n">
         <v>70</v>
@@ -2831,7 +2831,7 @@
         <v>12</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="F82" t="n">
         <v>5</v>
@@ -2861,7 +2861,7 @@
         <v>12</v>
       </c>
       <c r="E83" t="n">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="F83" t="n">
         <v>-2</v>
@@ -2891,7 +2891,7 @@
         <v>12</v>
       </c>
       <c r="E84" t="n">
-        <v>14</v>
+        <v>-14</v>
       </c>
       <c r="F84" t="n">
         <v>5</v>
@@ -2921,7 +2921,7 @@
         <v>24</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F85" t="n">
         <v>6</v>
@@ -2951,7 +2951,7 @@
         <v>18</v>
       </c>
       <c r="E86" t="n">
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="F86" t="n">
         <v>-1</v>
@@ -2981,7 +2981,7 @@
         <v>15</v>
       </c>
       <c r="E87" t="n">
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="F87" t="n">
         <v>9</v>
@@ -3011,7 +3011,7 @@
         <v>14</v>
       </c>
       <c r="E88" t="n">
-        <v>17</v>
+        <v>-17</v>
       </c>
       <c r="F88" t="n">
         <v>70</v>
@@ -3041,7 +3041,7 @@
         <v>20</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="F89" t="n">
         <v>8</v>
@@ -3071,7 +3071,7 @@
         <v>20</v>
       </c>
       <c r="E90" t="n">
-        <v>15</v>
+        <v>-15</v>
       </c>
       <c r="F90" t="n">
         <v>70</v>
@@ -3101,7 +3101,7 @@
         <v>20</v>
       </c>
       <c r="E91" t="n">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="F91" t="n">
         <v>70</v>
@@ -3183,7 +3183,7 @@
         <v>25</v>
       </c>
       <c r="E94" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F94" t="n">
         <v>70</v>
@@ -3243,7 +3243,7 @@
         <v>23</v>
       </c>
       <c r="E96" t="n">
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="F96" t="inlineStr"/>
       <c r="G96" t="inlineStr">
@@ -3271,7 +3271,7 @@
         <v>15</v>
       </c>
       <c r="E97" t="n">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="F97" t="n">
         <v>-3</v>
@@ -3301,7 +3301,7 @@
         <v>15</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="F98" t="n">
         <v>70</v>
@@ -3331,7 +3331,7 @@
         <v>15</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="F99" t="n">
         <v>70</v>
@@ -3385,7 +3385,7 @@
         <v>20</v>
       </c>
       <c r="E101" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F101" t="n">
         <v>11</v>
@@ -3415,7 +3415,7 @@
         <v>20</v>
       </c>
       <c r="E102" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F102" t="n">
         <v>11</v>
@@ -3445,7 +3445,7 @@
         <v>20</v>
       </c>
       <c r="E103" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="F103" t="n">
         <v>70</v>
@@ -3553,7 +3553,7 @@
         <v>10</v>
       </c>
       <c r="E107" t="n">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="F107" t="n">
         <v>6</v>
@@ -3583,7 +3583,7 @@
         <v>11</v>
       </c>
       <c r="E108" t="n">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="F108" t="n">
         <v>7</v>
@@ -3613,7 +3613,7 @@
         <v>16</v>
       </c>
       <c r="E109" t="n">
-        <v>17</v>
+        <v>-17</v>
       </c>
       <c r="F109" t="n">
         <v>-3</v>
@@ -3643,7 +3643,7 @@
         <v>12</v>
       </c>
       <c r="E110" t="n">
-        <v>15</v>
+        <v>-15</v>
       </c>
       <c r="F110" t="n">
         <v>-4</v>
@@ -3673,7 +3673,7 @@
         <v>21</v>
       </c>
       <c r="E111" t="n">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="F111" t="n">
         <v>5</v>
@@ -3763,7 +3763,7 @@
         <v>14</v>
       </c>
       <c r="E114" t="n">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="F114" t="n">
         <v>4</v>
@@ -3793,7 +3793,7 @@
         <v>14</v>
       </c>
       <c r="E115" t="n">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="F115" t="n">
         <v>70</v>
@@ -3823,7 +3823,7 @@
         <v>13</v>
       </c>
       <c r="E116" t="n">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="F116" t="n">
         <v>8</v>
@@ -3853,7 +3853,7 @@
         <v>13</v>
       </c>
       <c r="E117" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="F117" t="n">
         <v>9</v>
@@ -3907,7 +3907,7 @@
         <v>18</v>
       </c>
       <c r="E119" t="n">
-        <v>16</v>
+        <v>-16</v>
       </c>
       <c r="F119" t="n">
         <v>70</v>
@@ -3937,7 +3937,7 @@
         <v>11</v>
       </c>
       <c r="E120" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="F120" t="n">
         <v>8</v>
@@ -3967,7 +3967,7 @@
         <v>21</v>
       </c>
       <c r="E121" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="F121" t="n">
         <v>13</v>
@@ -3997,7 +3997,7 @@
         <v>16</v>
       </c>
       <c r="E122" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F122" t="n">
         <v>0</v>
@@ -4027,7 +4027,7 @@
         <v>17</v>
       </c>
       <c r="E123" t="n">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="F123" t="n">
         <v>70</v>
@@ -4079,7 +4079,7 @@
         <v>17</v>
       </c>
       <c r="E125" t="n">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="F125" t="n">
         <v>7</v>
@@ -4109,7 +4109,7 @@
         <v>20</v>
       </c>
       <c r="E126" t="n">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="F126" t="n">
         <v>4</v>
@@ -4139,7 +4139,7 @@
         <v>20</v>
       </c>
       <c r="E127" t="n">
-        <v>25</v>
+        <v>-25</v>
       </c>
       <c r="F127" t="n">
         <v>70</v>
@@ -4169,7 +4169,7 @@
         <v>20</v>
       </c>
       <c r="E128" t="n">
-        <v>26</v>
+        <v>-26</v>
       </c>
       <c r="F128" t="n">
         <v>70</v>
@@ -4199,7 +4199,7 @@
         <v>20</v>
       </c>
       <c r="E129" t="n">
-        <v>26</v>
+        <v>-26</v>
       </c>
       <c r="F129" t="n">
         <v>-15</v>
@@ -4229,7 +4229,7 @@
         <v>22</v>
       </c>
       <c r="E130" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F130" t="n">
         <v>0</v>
@@ -4259,7 +4259,7 @@
         <v>22</v>
       </c>
       <c r="E131" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F131" t="n">
         <v>0</v>
@@ -4289,7 +4289,7 @@
         <v>22</v>
       </c>
       <c r="E132" t="n">
-        <v>7</v>
+        <v>-7</v>
       </c>
       <c r="F132" t="n">
         <v>4</v>
@@ -4319,7 +4319,7 @@
         <v>22</v>
       </c>
       <c r="E133" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F133" t="n">
         <v>0</v>
@@ -4349,7 +4349,7 @@
         <v>22</v>
       </c>
       <c r="E134" t="n">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="F134" t="n">
         <v>0</v>
@@ -4379,7 +4379,7 @@
         <v>22</v>
       </c>
       <c r="E135" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="F135" t="n">
         <v>70</v>
@@ -4409,7 +4409,7 @@
         <v>22</v>
       </c>
       <c r="E136" t="n">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="F136" t="n">
         <v>9</v>

</xml_diff>